<commit_message>
Se crean apis y funciones parala descarga de excel en modulo de aprobados, rechazados y eventualidades. Se trabajara en un metodo general para la descargar de excel.
</commit_message>
<xml_diff>
--- a/WebAPI/wwwroot/Plantillas/EvidenciasMuestreoAprobados.xlsx
+++ b/WebAPI/wwwroot/Plantillas/EvidenciasMuestreoAprobados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nayeli Rojas\Documents\Plantillas_Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nayeli Rojas\Documents\SICA_INFOTEC\WebAPI\wwwroot\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -413,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,10 +476,10 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>